<commit_message>
modification à fiche de temps
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine3.xlsx
+++ b/FichesTemps/LouisGarceauSemaine3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C22CD9-6A97-45E7-BE67-2CE45F0429EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DFF791-8723-4AFA-B395-5E5DEC11A5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="864" yWindow="432" windowWidth="15960" windowHeight="9960" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="94">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -419,6 +419,15 @@
   </si>
   <si>
     <t>Utilisation du repository pattern de type d'analyse</t>
+  </si>
+  <si>
+    <t>Création de tests de Get, Create, Update et Delete de type d'analyse avec Moq et AutoFixture</t>
+  </si>
+  <si>
+    <t>Utilisation du repository pattern et création de tests de Get, Create, Update et Delete de type de valeur avec Moq et AutoFixture</t>
+  </si>
+  <si>
+    <t>Courte recherche sur les requêtes d'impression avec React Native</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -1805,7 +1814,7 @@
   <cols>
     <col min="1" max="1" width="13.5546875" customWidth="1"/>
     <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="100.21875" customWidth="1"/>
+    <col min="4" max="4" width="105.21875" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" style="33"/>
   </cols>
   <sheetData>
@@ -1891,7 +1900,7 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C11:C463)</f>
-        <v>19.75</v>
+        <v>20.8</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>64</v>
@@ -2101,16 +2110,28 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="45"/>
+      <c r="A28" s="42">
+        <v>44968</v>
+      </c>
       <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="46"/>
+      <c r="C28" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="45"/>
+      <c r="A29" s="42">
+        <v>44968</v>
+      </c>
       <c r="B29" s="46"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="46"/>
+      <c r="C29" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="45"/>
@@ -2119,10 +2140,16 @@
       <c r="D30" s="46"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="45"/>
+      <c r="A31" s="42">
+        <v>44969</v>
+      </c>
       <c r="B31" s="46"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="46"/>
+      <c r="C31" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="45"/>

</xml_diff>

<commit_message>
Début du visuel de résultat de requête et tentative du fix de test unitaire de création de requête
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine3.xlsx
+++ b/FichesTemps/LouisGarceauSemaine3.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DFF791-8723-4AFA-B395-5E5DEC11A5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587724D1-D4C6-471C-BAE6-321F91AD98AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="864" yWindow="432" windowWidth="15960" windowHeight="9960" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1524" yWindow="936" windowWidth="15960" windowHeight="9960" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temps" sheetId="15" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="99">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -428,6 +428,21 @@
   </si>
   <si>
     <t>Courte recherche sur les requêtes d'impression avec React Native</t>
+  </si>
+  <si>
+    <t>Recherche sur les requêtes d'impression avec React Native avec react-native-print et début de l'ajout au projet</t>
+  </si>
+  <si>
+    <t>Début de l'affichage des résultats d'une analyse</t>
+  </si>
+  <si>
+    <t>Continuation du travail sur l'affichage des résultats (fix de la liste des types de valeur)</t>
+  </si>
+  <si>
+    <t>Tentative de fix du test unitaire avec le nouveau code de création de requête</t>
+  </si>
+  <si>
+    <t>Fix du problème de object cycle dans le get de liste de types de valeur</t>
   </si>
 </sst>
 </file>
@@ -1806,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1900,7 +1915,7 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C11:C463)</f>
-        <v>20.8</v>
+        <v>24.3</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>64</v>
@@ -2152,34 +2167,64 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="45"/>
+      <c r="A32" s="42">
+        <v>44969</v>
+      </c>
       <c r="B32" s="46"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="46"/>
+      <c r="C32" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="D32" s="46" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="45"/>
+      <c r="A33" s="42">
+        <v>44969</v>
+      </c>
       <c r="B33" s="46"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="46"/>
+      <c r="C33" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="D33" s="46" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="42">
+        <v>44969</v>
+      </c>
       <c r="B34" s="46"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="46"/>
+      <c r="C34" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="46" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="42">
+        <v>44969</v>
+      </c>
       <c r="B35" s="46"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="46"/>
+      <c r="C35" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
+      <c r="A36" s="42">
+        <v>44969</v>
+      </c>
       <c r="B36" s="46"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="46"/>
+      <c r="C36" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="45"/>

</xml_diff>